<commit_message>
Added a character to Excel list for commit test
</commit_message>
<xml_diff>
--- a/Einkaufsliste.xlsx
+++ b/Einkaufsliste.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\OneDrive\Dokumente\Schule\SJ202526\NWT\gruene_wiese\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E17B66F-9509-458E-B65D-375E48EEFD87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,7 +59,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +336,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Kabellängen für EG und 1-3 berechnet
</commit_message>
<xml_diff>
--- a/Einkaufsliste.xlsx
+++ b/Einkaufsliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\OneDrive\Dokumente\Schule\SJ202526\NWT\gruene_wiese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB77674-2A4C-4B53-BA1E-874399EB1626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556DAB39-A7FC-4B22-8092-ED62DE18891F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagramm1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="21">
   <si>
     <t>Einkaufsliste</t>
   </si>
@@ -83,6 +83,24 @@
   <si>
     <t>EG (rechte Seite)</t>
   </si>
+  <si>
+    <t>EG (Zwischendecke links)</t>
+  </si>
+  <si>
+    <t>EG (Zwischendecke rechts)</t>
+  </si>
+  <si>
+    <t>1-3 (linke Seite)</t>
+  </si>
+  <si>
+    <t>1-3 (rechte Seite)</t>
+  </si>
+  <si>
+    <t>1-3 (Zwischendecke links)</t>
+  </si>
+  <si>
+    <t>1-3 (Zwischendecke rechts)</t>
+  </si>
 </sst>
 </file>
 
@@ -90,7 +108,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -150,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -288,13 +306,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -340,29 +439,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1479,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O45"/>
+  <dimension ref="B2:O103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView tabSelected="1" topLeftCell="J54" workbookViewId="0">
+      <selection activeCell="K67" sqref="K67:N67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1494,7 +1637,7 @@
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.77734375" customWidth="1"/>
     <col min="14" max="14" width="34.33203125" bestFit="1" customWidth="1"/>
@@ -1506,8 +1649,8 @@
         <v>0</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="L2" s="22"/>
-      <c r="O2" s="21"/>
+      <c r="L2" s="20"/>
+      <c r="O2" s="19"/>
     </row>
     <row r="5" spans="2:15" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
@@ -1537,7 +1680,7 @@
       <c r="N5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="24"/>
+      <c r="O5" s="22"/>
     </row>
     <row r="6" spans="2:15" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
@@ -1563,17 +1706,17 @@
       <c r="K6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="20">
+      <c r="L6" s="6">
         <v>1</v>
       </c>
       <c r="M6" s="12">
         <v>26</v>
       </c>
       <c r="N6" s="11">
-        <f>M6*L6</f>
+        <f t="shared" ref="N6:N18" si="0">M6*L6</f>
         <v>26</v>
       </c>
-      <c r="O6" s="23"/>
+      <c r="O6" s="21"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
@@ -1588,7 +1731,7 @@
       <c r="K7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="20">
+      <c r="L7" s="6">
         <v>3</v>
       </c>
       <c r="M7" s="12">
@@ -1596,10 +1739,10 @@
         <v>24</v>
       </c>
       <c r="N7" s="11">
-        <f>M7*L7</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="O7" s="23"/>
+      <c r="O7" s="21"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
@@ -1614,18 +1757,18 @@
       <c r="K8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="6">
         <v>2</v>
       </c>
       <c r="M8" s="12">
-        <f t="shared" ref="M8:M18" si="0">M7 - 2</f>
+        <f t="shared" ref="M8:M18" si="1">M7 - 2</f>
         <v>22</v>
       </c>
       <c r="N8" s="11">
-        <f>M8*L8</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="O8" s="23"/>
+      <c r="O8" s="21"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
@@ -1640,18 +1783,18 @@
       <c r="K9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="20">
+      <c r="L9" s="6">
         <v>2</v>
       </c>
       <c r="M9" s="12">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="N9" s="11">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="N9" s="11">
-        <f>M9*L9</f>
         <v>40</v>
       </c>
-      <c r="O9" s="23"/>
+      <c r="O9" s="21"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
@@ -1666,18 +1809,18 @@
       <c r="K10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="20">
+      <c r="L10" s="6">
         <v>1</v>
       </c>
       <c r="M10" s="12">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="N10" s="11">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="N10" s="11">
-        <f>M10*L10</f>
-        <v>18</v>
-      </c>
-      <c r="O10" s="23"/>
+      <c r="O10" s="21"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
@@ -1692,18 +1835,18 @@
       <c r="K11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="20">
+      <c r="L11" s="6">
         <v>1</v>
       </c>
       <c r="M11" s="12">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="N11" s="11">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="N11" s="11">
-        <f>M11*L11</f>
-        <v>16</v>
-      </c>
-      <c r="O11" s="23"/>
+      <c r="O11" s="21"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
@@ -1718,18 +1861,18 @@
       <c r="K12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="20">
+      <c r="L12" s="6">
         <v>2</v>
       </c>
       <c r="M12" s="12">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="N12" s="11">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="N12" s="11">
-        <f>M12*L12</f>
         <v>28</v>
       </c>
-      <c r="O12" s="23"/>
+      <c r="O12" s="21"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
@@ -1744,18 +1887,18 @@
       <c r="K13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="20">
+      <c r="L13" s="6">
         <v>2</v>
       </c>
       <c r="M13" s="12">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="N13" s="11">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="N13" s="11">
-        <f>M13*L13</f>
         <v>24</v>
       </c>
-      <c r="O13" s="23"/>
+      <c r="O13" s="21"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
@@ -1770,18 +1913,18 @@
       <c r="K14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="20">
+      <c r="L14" s="6">
         <v>2</v>
       </c>
       <c r="M14" s="12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N14" s="11">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="N14" s="11">
-        <f>M14*L14</f>
         <v>20</v>
       </c>
-      <c r="O14" s="23"/>
+      <c r="O14" s="21"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
@@ -1796,18 +1939,18 @@
       <c r="K15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L15" s="20">
+      <c r="L15" s="6">
         <v>2</v>
       </c>
       <c r="M15" s="12">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="N15" s="11">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="N15" s="11">
-        <f>M15*L15</f>
         <v>16</v>
       </c>
-      <c r="O15" s="23"/>
+      <c r="O15" s="21"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
@@ -1822,18 +1965,18 @@
       <c r="K16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L16" s="20">
+      <c r="L16" s="6">
         <v>3</v>
       </c>
       <c r="M16" s="12">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="N16" s="11">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="N16" s="11">
-        <f>M16*L16</f>
         <v>18</v>
       </c>
-      <c r="O16" s="23"/>
+      <c r="O16" s="21"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
@@ -1848,18 +1991,18 @@
       <c r="K17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="20">
+      <c r="L17" s="6">
         <v>3</v>
       </c>
       <c r="M17" s="12">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="N17" s="11">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="N17" s="11">
-        <f>M17*L17</f>
         <v>12</v>
       </c>
-      <c r="O17" s="23"/>
+      <c r="O17" s="21"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
@@ -1871,21 +2014,21 @@
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="29" t="s">
+      <c r="K18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="L18" s="26">
+      <c r="L18" s="23">
         <v>3</v>
       </c>
-      <c r="M18" s="27">
+      <c r="M18" s="24">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N18" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="N18" s="28">
-        <f>M18*L18</f>
         <v>6</v>
       </c>
-      <c r="O18" s="23"/>
+      <c r="O18" s="21"/>
     </row>
     <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="14"/>
@@ -1897,17 +2040,20 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="29" t="s">
         <v>14</v>
+      </c>
+      <c r="L19" s="27">
+        <v>4</v>
       </c>
       <c r="M19" s="11">
         <v>22</v>
       </c>
       <c r="N19" s="11">
-        <f t="shared" ref="N19:N45" si="1">M19*L19</f>
-        <v>0</v>
-      </c>
-      <c r="O19" s="19"/>
+        <f t="shared" ref="N19:N45" si="2">M19*L19</f>
+        <v>88</v>
+      </c>
+      <c r="O19" s="10"/>
     </row>
     <row r="20" spans="2:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
@@ -1924,203 +2070,983 @@
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
+      <c r="K20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="10">
+        <v>3</v>
+      </c>
       <c r="M20" s="11">
         <f>M19-2</f>
         <v>20</v>
       </c>
       <c r="N20" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="19"/>
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="O20" s="10"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G21" s="17"/>
+      <c r="K21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="27">
+        <v>3</v>
+      </c>
       <c r="M21" s="11">
-        <f t="shared" ref="M21:M30" si="2">M20-2</f>
+        <f t="shared" ref="M21:M29" si="3">M20-2</f>
         <v>18</v>
       </c>
       <c r="N21" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="25"/>
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="27">
+        <v>3</v>
+      </c>
       <c r="M22" s="11">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="N22" s="11">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="27">
+        <v>3</v>
+      </c>
+      <c r="M23" s="11">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="N23" s="11">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" s="27">
+        <v>2</v>
+      </c>
+      <c r="M24" s="11">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="N24" s="11">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25" s="27">
+        <v>1</v>
+      </c>
+      <c r="M25" s="11">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="N25" s="11">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L26" s="27">
+        <v>2</v>
+      </c>
+      <c r="M26" s="11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="N26" s="11">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N22" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="25"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="M23" s="11">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N23" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="25"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="M24" s="11">
+      <c r="L27" s="27">
+        <v>2</v>
+      </c>
+      <c r="M27" s="11">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="N27" s="11">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N24" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="25"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="M25" s="11">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="N25" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="M26" s="11">
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L28" s="27">
+        <v>2</v>
+      </c>
+      <c r="M28" s="11">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="N28" s="11">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="N26" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="M27" s="11">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="N27" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="M28" s="11">
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K29" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="28">
+        <v>2</v>
+      </c>
+      <c r="M29" s="25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="N29" s="25">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N28" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="M29" s="11">
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K30" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="27">
+        <v>11</v>
+      </c>
+      <c r="M30" s="33">
+        <v>6</v>
+      </c>
+      <c r="N30" s="31">
+        <f>L30*M30</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K31" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="L31" s="27">
+        <v>10</v>
+      </c>
+      <c r="M31" s="34">
+        <f>M30-2</f>
+        <v>4</v>
+      </c>
+      <c r="N31" s="31">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="N29" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="N31" s="11"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="N32" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="K32" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="L32" s="28">
+        <v>11</v>
+      </c>
+      <c r="M32" s="35">
+        <f t="shared" ref="M32:M35" si="4">M31-2</f>
+        <v>2</v>
+      </c>
+      <c r="N32" s="23">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K33" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" s="36">
+        <v>8</v>
+      </c>
+      <c r="M33" s="27">
+        <v>6</v>
+      </c>
       <c r="N33" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K34" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" s="12">
+        <v>6</v>
+      </c>
+      <c r="M34" s="27">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
       <c r="N34" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N35" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="14:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="11:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K35" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" s="38">
+        <v>9</v>
+      </c>
+      <c r="M35" s="39">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="N35" s="40">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K36" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="41">
+        <v>7</v>
+      </c>
+      <c r="M36" s="10">
+        <v>26</v>
+      </c>
       <c r="N36" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="14:14" x14ac:dyDescent="0.3">
+        <f>L36*M36*3</f>
+        <v>546</v>
+      </c>
+    </row>
+    <row r="37" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K37" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L37" s="12">
+        <v>2</v>
+      </c>
+      <c r="M37" s="10">
+        <v>24</v>
+      </c>
       <c r="N37" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="14:14" x14ac:dyDescent="0.3">
+        <f t="shared" ref="N37:N48" si="5">L37*M37*3</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K38" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L38" s="12">
+        <v>2</v>
+      </c>
+      <c r="M38" s="10">
+        <f>M37-2</f>
+        <v>22</v>
+      </c>
       <c r="N38" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="14:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K39" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L39" s="12">
+        <v>3</v>
+      </c>
+      <c r="M39" s="10">
+        <f t="shared" ref="M39:M48" si="6">M38-2</f>
+        <v>20</v>
+      </c>
       <c r="N39" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="14:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K40" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L40" s="12">
+        <v>2</v>
+      </c>
+      <c r="M40" s="10">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
       <c r="N40" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="14:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K41" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L41" s="12">
+        <v>2</v>
+      </c>
+      <c r="M41" s="10">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
       <c r="N41" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="14:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K42" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L42" s="12">
+        <v>2</v>
+      </c>
+      <c r="M42" s="10">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
       <c r="N42" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="14:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K43" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L43" s="12">
+        <v>3</v>
+      </c>
+      <c r="M43" s="10">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
       <c r="N43" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="14:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K44" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L44" s="12">
+        <v>2</v>
+      </c>
+      <c r="M44" s="10">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
       <c r="N44" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="14:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K45" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L45" s="12">
+        <v>2</v>
+      </c>
+      <c r="M45" s="10">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
       <c r="N45" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K46" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L46" s="12">
+        <v>2</v>
+      </c>
+      <c r="M46" s="10">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="N46" s="11">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K47" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="L47" s="12">
+        <v>3</v>
+      </c>
+      <c r="M47" s="10">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="N47" s="11">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K48" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L48" s="24">
+        <v>3</v>
+      </c>
+      <c r="M48" s="23">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="N48" s="25">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K49" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L49" s="29">
+        <v>5</v>
+      </c>
+      <c r="M49" s="33">
+        <v>26</v>
+      </c>
+      <c r="N49" s="10">
+        <f>L49*M49*3</f>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="50" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K50" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L50" s="6">
+        <v>2</v>
+      </c>
+      <c r="M50" s="12">
+        <f>M49-2</f>
+        <v>24</v>
+      </c>
+      <c r="N50" s="10">
+        <f t="shared" ref="N50:N67" si="7">L50*M50*3</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L51" s="6">
+        <v>2</v>
+      </c>
+      <c r="M51" s="12">
+        <f t="shared" ref="M51:M60" si="8">M50-2</f>
+        <v>22</v>
+      </c>
+      <c r="N51" s="10">
+        <f t="shared" si="7"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K52" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L52" s="6">
+        <v>2</v>
+      </c>
+      <c r="M52" s="12">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="N52" s="10">
+        <f t="shared" si="7"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K53" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L53" s="6">
+        <v>2</v>
+      </c>
+      <c r="M53" s="12">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="N53" s="10">
+        <f t="shared" si="7"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K54" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L54" s="6">
+        <v>2</v>
+      </c>
+      <c r="M54" s="12">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="N54" s="10">
+        <f t="shared" si="7"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K55" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L55" s="6">
+        <v>2</v>
+      </c>
+      <c r="M55" s="12">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="N55" s="10">
+        <f t="shared" si="7"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K56" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L56" s="6">
+        <v>3</v>
+      </c>
+      <c r="M56" s="12">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="N56" s="10">
+        <f t="shared" si="7"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K57" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L57" s="6">
+        <v>2</v>
+      </c>
+      <c r="M57" s="12">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="N57" s="10">
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K58" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L58" s="6">
+        <v>2</v>
+      </c>
+      <c r="M58" s="12">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="N58" s="10">
+        <f t="shared" si="7"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L59" s="6">
+        <v>2</v>
+      </c>
+      <c r="M59" s="12">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="N59" s="10">
+        <f t="shared" si="7"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K60" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L60" s="6">
+        <v>2</v>
+      </c>
+      <c r="M60" s="12">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="N60" s="10">
+        <f t="shared" si="7"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K61" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="L61" s="26">
+        <v>2</v>
+      </c>
+      <c r="M61" s="24">
+        <f>M60-2</f>
+        <v>2</v>
+      </c>
+      <c r="N61" s="23">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K62" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="L62" s="10">
+        <v>13</v>
+      </c>
+      <c r="M62" s="12">
+        <v>6</v>
+      </c>
+      <c r="N62" s="10">
+        <f t="shared" si="7"/>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K63" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L63" s="10">
+        <v>9</v>
+      </c>
+      <c r="M63" s="12">
+        <f t="shared" ref="M62:M67" si="9">M62-2</f>
+        <v>4</v>
+      </c>
+      <c r="N63" s="10">
+        <f t="shared" si="7"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K64" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L64" s="23">
+        <v>10</v>
+      </c>
+      <c r="M64" s="24">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="N64" s="23">
+        <f t="shared" si="7"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K65" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L65" s="10">
+        <v>10</v>
+      </c>
+      <c r="M65" s="12">
+        <v>6</v>
+      </c>
+      <c r="N65" s="10">
+        <f t="shared" si="7"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K66" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L66" s="10">
+        <v>6</v>
+      </c>
+      <c r="M66" s="12">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="N66" s="10">
+        <f t="shared" si="7"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="11:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K67" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="L67" s="43">
+        <v>6</v>
+      </c>
+      <c r="M67" s="38">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="N67" s="43">
+        <f t="shared" si="7"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K68" s="10"/>
+      <c r="L68" s="10"/>
+      <c r="M68" s="10"/>
+      <c r="N68" s="10"/>
+    </row>
+    <row r="69" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+    </row>
+    <row r="70" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K70" s="10"/>
+      <c r="L70" s="10"/>
+      <c r="M70" s="10"/>
+      <c r="N70" s="10"/>
+    </row>
+    <row r="71" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K71" s="10"/>
+      <c r="L71" s="10"/>
+      <c r="M71" s="10"/>
+      <c r="N71" s="10"/>
+    </row>
+    <row r="72" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
+      <c r="M72" s="10"/>
+      <c r="N72" s="10"/>
+    </row>
+    <row r="73" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K73" s="10"/>
+      <c r="L73" s="10"/>
+      <c r="M73" s="10"/>
+      <c r="N73" s="10"/>
+    </row>
+    <row r="74" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K74" s="10"/>
+      <c r="L74" s="10"/>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+    </row>
+    <row r="75" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="M75" s="10"/>
+      <c r="N75" s="10"/>
+    </row>
+    <row r="76" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K76" s="10"/>
+      <c r="L76" s="10"/>
+      <c r="M76" s="10"/>
+      <c r="N76" s="10"/>
+    </row>
+    <row r="77" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K77" s="10"/>
+      <c r="L77" s="10"/>
+      <c r="M77" s="10"/>
+      <c r="N77" s="10"/>
+    </row>
+    <row r="78" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K78" s="10"/>
+      <c r="L78" s="10"/>
+      <c r="M78" s="10"/>
+      <c r="N78" s="10"/>
+    </row>
+    <row r="79" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K79" s="10"/>
+      <c r="L79" s="10"/>
+      <c r="M79" s="10"/>
+      <c r="N79" s="10"/>
+    </row>
+    <row r="80" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K80" s="10"/>
+      <c r="L80" s="10"/>
+      <c r="M80" s="10"/>
+      <c r="N80" s="10"/>
+    </row>
+    <row r="81" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K81" s="10"/>
+      <c r="L81" s="10"/>
+      <c r="M81" s="10"/>
+      <c r="N81" s="10"/>
+    </row>
+    <row r="82" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K82" s="10"/>
+      <c r="L82" s="10"/>
+      <c r="M82" s="10"/>
+      <c r="N82" s="10"/>
+    </row>
+    <row r="83" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K83" s="10"/>
+      <c r="L83" s="10"/>
+      <c r="M83" s="10"/>
+      <c r="N83" s="10"/>
+    </row>
+    <row r="84" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K84" s="10"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
+      <c r="N84" s="10"/>
+    </row>
+    <row r="85" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K85" s="10"/>
+      <c r="L85" s="10"/>
+      <c r="M85" s="10"/>
+      <c r="N85" s="10"/>
+    </row>
+    <row r="86" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K86" s="10"/>
+      <c r="L86" s="10"/>
+      <c r="M86" s="10"/>
+      <c r="N86" s="10"/>
+    </row>
+    <row r="87" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K87" s="10"/>
+      <c r="L87" s="10"/>
+      <c r="M87" s="10"/>
+      <c r="N87" s="10"/>
+    </row>
+    <row r="88" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K88" s="10"/>
+      <c r="L88" s="10"/>
+      <c r="M88" s="10"/>
+      <c r="N88" s="10"/>
+    </row>
+    <row r="89" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="10"/>
+      <c r="N89" s="10"/>
+    </row>
+    <row r="90" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="10"/>
+    </row>
+    <row r="91" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="10"/>
+      <c r="N91" s="10"/>
+    </row>
+    <row r="92" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K92" s="10"/>
+      <c r="L92" s="10"/>
+      <c r="M92" s="10"/>
+      <c r="N92" s="10"/>
+    </row>
+    <row r="93" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K93" s="10"/>
+      <c r="L93" s="10"/>
+      <c r="M93" s="10"/>
+      <c r="N93" s="10"/>
+    </row>
+    <row r="94" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="10"/>
+      <c r="N94" s="10"/>
+    </row>
+    <row r="95" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K95" s="10"/>
+      <c r="L95" s="10"/>
+      <c r="M95" s="10"/>
+      <c r="N95" s="10"/>
+    </row>
+    <row r="96" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K96" s="10"/>
+      <c r="L96" s="10"/>
+      <c r="M96" s="10"/>
+      <c r="N96" s="10"/>
+    </row>
+    <row r="97" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K97" s="10"/>
+      <c r="L97" s="10"/>
+      <c r="M97" s="10"/>
+      <c r="N97" s="10"/>
+    </row>
+    <row r="98" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K98" s="10"/>
+      <c r="L98" s="10"/>
+      <c r="M98" s="10"/>
+      <c r="N98" s="10"/>
+    </row>
+    <row r="99" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K99" s="10"/>
+      <c r="L99" s="10"/>
+      <c r="M99" s="10"/>
+      <c r="N99" s="10"/>
+    </row>
+    <row r="100" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K100" s="10"/>
+      <c r="L100" s="10"/>
+      <c r="M100" s="10"/>
+      <c r="N100" s="10"/>
+    </row>
+    <row r="101" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K101" s="10"/>
+      <c r="L101" s="10"/>
+      <c r="M101" s="10"/>
+      <c r="N101" s="10"/>
+    </row>
+    <row r="102" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K102" s="10"/>
+      <c r="L102" s="10"/>
+      <c r="M102" s="10"/>
+      <c r="N102" s="10"/>
+    </row>
+    <row r="103" spans="11:14" x14ac:dyDescent="0.3">
+      <c r="K103" s="10"/>
+      <c r="L103" s="10"/>
+      <c r="M103" s="10"/>
+      <c r="N103" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Kabelkanäle und Trassen im Excel berechnet
</commit_message>
<xml_diff>
--- a/Einkaufsliste.xlsx
+++ b/Einkaufsliste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\Schule\NWT\gruene_wiese\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cleme\OneDrive\Dokumente\Schule\SJ202526\NWT\gruene_wiese\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A347773B-C0B6-4EB0-8395-EB2E35368978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5893C51-0F11-4D7A-8A2C-BD3E917EF590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagramm1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="38">
   <si>
     <t>Einkaufsliste</t>
   </si>
@@ -116,6 +116,42 @@
   <si>
     <t>Gesamt (mit 7.5% Reserve):</t>
   </si>
+  <si>
+    <t>Kabelkanäle</t>
+  </si>
+  <si>
+    <t>EG (Zwischendecke WC)</t>
+  </si>
+  <si>
+    <t>1.Stockwerk - 3. Stockwerk</t>
+  </si>
+  <si>
+    <t>1.-3. (Zwischendecke)</t>
+  </si>
+  <si>
+    <t>DG (linke Seite)</t>
+  </si>
+  <si>
+    <t>DG (rechte Seite)</t>
+  </si>
+  <si>
+    <t>DG (Zwischendecke links)</t>
+  </si>
+  <si>
+    <t>DG (Zwischendecke rechts)</t>
+  </si>
+  <si>
+    <t>Gesamt mit Reserve (7.5%):</t>
+  </si>
+  <si>
+    <t>https://www.reichelt.at/at/de/shop/produkt/cat_6_netzwerkkabel_s_ftp_grau_305_m-350271</t>
+  </si>
+  <si>
+    <t>Cat.6 Netzwerkkabel, S/FTP, grau, 305 m</t>
+  </si>
+  <si>
+    <t>Kabeltrassen</t>
+  </si>
 </sst>
 </file>
 
@@ -124,9 +160,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +211,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="17"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -184,7 +227,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -414,13 +457,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -508,14 +582,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Prozent" xfId="2" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -533,7 +643,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1625,29 +1735,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O103"/>
+  <dimension ref="B2:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H76" workbookViewId="0">
-      <selection activeCell="O92" sqref="O92"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" customWidth="1"/>
-    <col min="2" max="2" width="90.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="9.1328125" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="90.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9.109375" customWidth="1"/>
+    <col min="11" max="11" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.46484375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="32.25" x14ac:dyDescent="0.95">
+    <row r="2" spans="2:20" ht="32.4" x14ac:dyDescent="0.6">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1655,7 +1770,23 @@
       <c r="L2" s="20"/>
       <c r="O2" s="19"/>
     </row>
-    <row r="5" spans="2:15" ht="19.899999999999999" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="2:20" ht="22.2" x14ac:dyDescent="0.45">
+      <c r="K3" s="36"/>
+      <c r="P3" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+    </row>
+    <row r="5" spans="2:20" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
@@ -1684,8 +1815,21 @@
         <v>12</v>
       </c>
       <c r="O5" s="22"/>
-    </row>
-    <row r="6" spans="2:15" ht="28.9" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="P5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R5" s="38"/>
+      <c r="S5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1720,13 +1864,37 @@
         <v>26</v>
       </c>
       <c r="O6" s="21"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
+      <c r="P6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="37">
+        <v>7</v>
+      </c>
+      <c r="R6" s="37"/>
+      <c r="S6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="T6" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="6">
+        <v>25</v>
+      </c>
+      <c r="E7" s="10">
+        <v>282.3</v>
+      </c>
+      <c r="F7" s="11">
+        <f>PRODUCT(D7,E7)</f>
+        <v>7057.5</v>
+      </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -1746,8 +1914,21 @@
         <v>72</v>
       </c>
       <c r="O7" s="21"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P7" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>11</v>
+      </c>
+      <c r="R7" s="37"/>
+      <c r="S7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="T7" s="37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1772,8 +1953,21 @@
         <v>44</v>
       </c>
       <c r="O8" s="21"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P8" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="23">
+        <v>7</v>
+      </c>
+      <c r="R8" s="37"/>
+      <c r="S8" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="T8" s="23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1798,8 +1992,22 @@
         <v>40</v>
       </c>
       <c r="O9" s="21"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q9" s="37">
+        <v>7</v>
+      </c>
+      <c r="R9" s="37"/>
+      <c r="S9" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9" s="45">
+        <f>35*3</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -1824,8 +2032,21 @@
         <v>18</v>
       </c>
       <c r="O10" s="21"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="37">
+        <v>11</v>
+      </c>
+      <c r="R10" s="37"/>
+      <c r="S10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" s="25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -1850,8 +2071,21 @@
         <v>16</v>
       </c>
       <c r="O11" s="21"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P11" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="23">
+        <v>5</v>
+      </c>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="T11" s="11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -1876,8 +2110,22 @@
         <v>28</v>
       </c>
       <c r="O12" s="21"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P12" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="37">
+        <f>7*6</f>
+        <v>42</v>
+      </c>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="T12" s="46">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1902,8 +2150,23 @@
         <v>24</v>
       </c>
       <c r="O13" s="21"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P13" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="37">
+        <f>11*6</f>
+        <v>66</v>
+      </c>
+      <c r="R13" s="37"/>
+      <c r="S13" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="T13" s="48">
+        <f>SUM(T6:T12)</f>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1928,8 +2191,23 @@
         <v>20</v>
       </c>
       <c r="O14" s="21"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P14" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q14" s="25">
+        <f>7*6</f>
+        <v>42</v>
+      </c>
+      <c r="R14" s="37"/>
+      <c r="S14" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="T14" s="37">
+        <f>T13 + T13 * 0.075</f>
+        <v>360.125</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1954,8 +2232,17 @@
         <v>16</v>
       </c>
       <c r="O15" s="21"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P15" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>7</v>
+      </c>
+      <c r="R15" s="37"/>
+      <c r="S15" s="50"/>
+      <c r="T15" s="37"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1980,8 +2267,17 @@
         <v>18</v>
       </c>
       <c r="O16" s="21"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P16" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>11</v>
+      </c>
+      <c r="R16" s="37"/>
+      <c r="S16" s="50"/>
+      <c r="T16" s="37"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2006,8 +2302,17 @@
         <v>12</v>
       </c>
       <c r="O17" s="21"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q17" s="25">
+        <v>7</v>
+      </c>
+      <c r="R17" s="37"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="37"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -2032,8 +2337,17 @@
         <v>6</v>
       </c>
       <c r="O18" s="21"/>
-    </row>
-    <row r="19" spans="2:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="P18" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>4</v>
+      </c>
+      <c r="R18" s="39"/>
+      <c r="S18" s="39"/>
+      <c r="T18" s="39"/>
+    </row>
+    <row r="19" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
@@ -2057,15 +2371,24 @@
         <v>88</v>
       </c>
       <c r="O19" s="10"/>
-    </row>
-    <row r="20" spans="2:15" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="P19" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>5</v>
+      </c>
+      <c r="R19" s="39"/>
+      <c r="S19" s="39"/>
+      <c r="T19" s="39"/>
+    </row>
+    <row r="20" spans="2:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="10"/>
       <c r="F20" s="11">
         <f>SUM(F6:F19)</f>
-        <v>1700</v>
+        <v>8757.5</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>3</v>
@@ -2088,8 +2411,17 @@
         <v>60</v>
       </c>
       <c r="O20" s="10"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P20" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>8</v>
+      </c>
+      <c r="R20" s="39"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G21" s="17"/>
       <c r="K21" s="6" t="s">
         <v>14</v>
@@ -2105,8 +2437,17 @@
         <f t="shared" si="2"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P21" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q21" s="25">
+        <v>7</v>
+      </c>
+      <c r="R21" s="39"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+    </row>
+    <row r="22" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K22" s="6" t="s">
         <v>14</v>
       </c>
@@ -2121,8 +2462,18 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P22" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q22" s="31">
+        <f>SUM(Q6:Q21)</f>
+        <v>247</v>
+      </c>
+      <c r="R22" s="39"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="K23" s="6" t="s">
         <v>14</v>
       </c>
@@ -2137,8 +2488,18 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P23" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q23" s="37">
+        <f>Q22 + Q22 * 0.075</f>
+        <v>265.52499999999998</v>
+      </c>
+      <c r="R23" s="39"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="K24" s="6" t="s">
         <v>14</v>
       </c>
@@ -2153,8 +2514,11 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="R24" s="39"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="K25" s="6" t="s">
         <v>14</v>
       </c>
@@ -2169,8 +2533,11 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="R25" s="39"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="K26" s="6" t="s">
         <v>14</v>
       </c>
@@ -2185,8 +2552,13 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="39"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="37"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="K27" s="6" t="s">
         <v>14</v>
       </c>
@@ -2201,8 +2573,13 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="39"/>
+      <c r="S27" s="39"/>
+      <c r="T27" s="39"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="K28" s="6" t="s">
         <v>14</v>
       </c>
@@ -2217,8 +2594,11 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P28" s="37"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="39"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="K29" s="26" t="s">
         <v>14</v>
       </c>
@@ -2233,8 +2613,9 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="R29" s="39"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="K30" s="6" t="s">
         <v>15</v>
       </c>
@@ -2248,8 +2629,9 @@
         <f>L30*M30</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="R30" s="39"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="K31" s="6" t="s">
         <v>15</v>
       </c>
@@ -2264,8 +2646,12 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.45">
+      <c r="P31" s="37"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="39"/>
+      <c r="S31" s="39"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="K32" s="26" t="s">
         <v>15</v>
       </c>
@@ -2280,8 +2666,12 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="11:14" x14ac:dyDescent="0.45">
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="39"/>
+      <c r="S32" s="39"/>
+    </row>
+    <row r="33" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K33" s="6" t="s">
         <v>16</v>
       </c>
@@ -2295,8 +2685,12 @@
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="34" spans="11:14" x14ac:dyDescent="0.45">
+      <c r="P33" s="39"/>
+      <c r="Q33" s="39"/>
+      <c r="R33" s="39"/>
+      <c r="S33" s="39"/>
+    </row>
+    <row r="34" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K34" s="6" t="s">
         <v>16</v>
       </c>
@@ -2311,8 +2705,12 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="11:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="P34" s="39"/>
+      <c r="Q34" s="39"/>
+      <c r="R34" s="39"/>
+      <c r="S34" s="39"/>
+    </row>
+    <row r="35" spans="11:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K35" s="29" t="s">
         <v>16</v>
       </c>
@@ -2327,8 +2725,12 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="11:14" x14ac:dyDescent="0.45">
+      <c r="P35" s="39"/>
+      <c r="Q35" s="39"/>
+      <c r="R35" s="39"/>
+      <c r="S35" s="39"/>
+    </row>
+    <row r="36" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K36" s="6" t="s">
         <v>17</v>
       </c>
@@ -2342,8 +2744,12 @@
         <f>L36*M36*3+30</f>
         <v>576</v>
       </c>
-    </row>
-    <row r="37" spans="11:14" x14ac:dyDescent="0.45">
+      <c r="P36" s="39"/>
+      <c r="Q36" s="39"/>
+      <c r="R36" s="39"/>
+      <c r="S36" s="39"/>
+    </row>
+    <row r="37" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K37" s="6" t="s">
         <v>17</v>
       </c>
@@ -2358,7 +2764,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="38" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="38" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K38" s="6" t="s">
         <v>17</v>
       </c>
@@ -2374,7 +2780,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="39" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K39" s="6" t="s">
         <v>17</v>
       </c>
@@ -2390,7 +2796,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="40" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K40" s="6" t="s">
         <v>17</v>
       </c>
@@ -2406,7 +2812,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="41" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K41" s="6" t="s">
         <v>17</v>
       </c>
@@ -2422,7 +2828,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="42" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K42" s="6" t="s">
         <v>17</v>
       </c>
@@ -2438,7 +2844,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="43" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K43" s="6" t="s">
         <v>17</v>
       </c>
@@ -2454,7 +2860,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="44" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K44" s="6" t="s">
         <v>17</v>
       </c>
@@ -2470,7 +2876,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="45" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K45" s="6" t="s">
         <v>17</v>
       </c>
@@ -2486,7 +2892,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="46" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K46" s="6" t="s">
         <v>17</v>
       </c>
@@ -2502,7 +2908,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="47" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K47" s="6" t="s">
         <v>17</v>
       </c>
@@ -2518,7 +2924,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="48" spans="11:19" x14ac:dyDescent="0.3">
       <c r="K48" s="26" t="s">
         <v>17</v>
       </c>
@@ -2534,7 +2940,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="49" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K49" s="6" t="s">
         <v>18</v>
       </c>
@@ -2549,7 +2955,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="50" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="50" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K50" s="6" t="s">
         <v>18</v>
       </c>
@@ -2565,7 +2971,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="51" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K51" s="6" t="s">
         <v>18</v>
       </c>
@@ -2581,7 +2987,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="52" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K52" s="6" t="s">
         <v>18</v>
       </c>
@@ -2597,7 +3003,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="53" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K53" s="6" t="s">
         <v>18</v>
       </c>
@@ -2613,7 +3019,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="54" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K54" s="6" t="s">
         <v>18</v>
       </c>
@@ -2629,7 +3035,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="55" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K55" s="6" t="s">
         <v>18</v>
       </c>
@@ -2645,7 +3051,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="56" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K56" s="6" t="s">
         <v>18</v>
       </c>
@@ -2661,7 +3067,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="57" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="57" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K57" s="6" t="s">
         <v>18</v>
       </c>
@@ -2677,7 +3083,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="58" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K58" s="6" t="s">
         <v>18</v>
       </c>
@@ -2693,7 +3099,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="59" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K59" s="6" t="s">
         <v>18</v>
       </c>
@@ -2709,7 +3115,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="60" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K60" s="6" t="s">
         <v>18</v>
       </c>
@@ -2725,7 +3131,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="61" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="61" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K61" s="26" t="s">
         <v>18</v>
       </c>
@@ -2741,7 +3147,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="62" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K62" s="27" t="s">
         <v>19</v>
       </c>
@@ -2756,7 +3162,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="63" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="63" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K63" s="6" t="s">
         <v>19</v>
       </c>
@@ -2772,7 +3178,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="64" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K64" s="26" t="s">
         <v>19</v>
       </c>
@@ -2788,7 +3194,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="65" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K65" s="6" t="s">
         <v>20</v>
       </c>
@@ -2803,7 +3209,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="66" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="66" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K66" s="6" t="s">
         <v>20</v>
       </c>
@@ -2819,7 +3225,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="11:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="11:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K67" s="29" t="s">
         <v>20</v>
       </c>
@@ -2835,7 +3241,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="68" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K68" s="10" t="s">
         <v>21</v>
       </c>
@@ -2850,7 +3256,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="69" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="69" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K69" s="10" t="s">
         <v>21</v>
       </c>
@@ -2866,7 +3272,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="70" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="70" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K70" s="10" t="s">
         <v>21</v>
       </c>
@@ -2882,7 +3288,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="71" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K71" s="10" t="s">
         <v>21</v>
       </c>
@@ -2898,7 +3304,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="72" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K72" s="10" t="s">
         <v>21</v>
       </c>
@@ -2914,7 +3320,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="73" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K73" s="10" t="s">
         <v>21</v>
       </c>
@@ -2930,7 +3336,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="74" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K74" s="10" t="s">
         <v>21</v>
       </c>
@@ -2946,7 +3352,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="75" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="75" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K75" s="10" t="s">
         <v>21</v>
       </c>
@@ -2962,7 +3368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="76" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K76" s="10" t="s">
         <v>21</v>
       </c>
@@ -2978,7 +3384,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="77" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K77" s="10" t="s">
         <v>21</v>
       </c>
@@ -2994,7 +3400,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="78" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="78" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K78" s="10" t="s">
         <v>21</v>
       </c>
@@ -3010,7 +3416,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="79" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K79" s="10" t="s">
         <v>21</v>
       </c>
@@ -3026,7 +3432,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="80" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K80" s="23" t="s">
         <v>21</v>
       </c>
@@ -3042,7 +3448,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="81" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K81" s="10" t="s">
         <v>22</v>
       </c>
@@ -3057,7 +3463,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="82" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K82" s="10" t="s">
         <v>22</v>
       </c>
@@ -3073,7 +3479,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="83" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K83" s="10" t="s">
         <v>22</v>
       </c>
@@ -3089,7 +3495,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="84" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K84" s="10" t="s">
         <v>22</v>
       </c>
@@ -3105,7 +3511,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="85" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="85" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K85" s="10" t="s">
         <v>22</v>
       </c>
@@ -3121,7 +3527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="86" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K86" s="10" t="s">
         <v>22</v>
       </c>
@@ -3137,7 +3543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="87" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K87" s="10" t="s">
         <v>22</v>
       </c>
@@ -3153,7 +3559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="88" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K88" s="10" t="s">
         <v>22</v>
       </c>
@@ -3168,7 +3574,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="89" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K89" s="23" t="s">
         <v>22</v>
       </c>
@@ -3183,7 +3589,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="90" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K90" s="10" t="s">
         <v>23</v>
       </c>
@@ -3198,7 +3604,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="91" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K91" s="10" t="s">
         <v>23</v>
       </c>
@@ -3213,7 +3619,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="92" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="92" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K92" s="10" t="s">
         <v>23</v>
       </c>
@@ -3228,7 +3634,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="93" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="93" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K93" s="10" t="s">
         <v>23</v>
       </c>
@@ -3243,7 +3649,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="94" spans="11:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="94" spans="11:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K94" s="31" t="s">
         <v>23</v>
       </c>
@@ -3258,7 +3664,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="95" spans="11:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="11:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K95" s="15" t="s">
         <v>24</v>
       </c>
@@ -3274,49 +3680,49 @@
         <v>7274.5249999999996</v>
       </c>
     </row>
-    <row r="96" spans="11:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="11:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="K96" s="10"/>
       <c r="L96" s="10"/>
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
     </row>
-    <row r="97" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="97" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K97" s="10"/>
       <c r="L97" s="10"/>
       <c r="M97" s="10"/>
       <c r="N97" s="10"/>
     </row>
-    <row r="98" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="98" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K98" s="10"/>
       <c r="L98" s="10"/>
       <c r="M98" s="10"/>
       <c r="N98" s="10"/>
     </row>
-    <row r="99" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="99" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K99" s="10"/>
       <c r="L99" s="10"/>
       <c r="M99" s="10"/>
       <c r="N99" s="10"/>
     </row>
-    <row r="100" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="100" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K100" s="10"/>
       <c r="L100" s="10"/>
       <c r="M100" s="10"/>
       <c r="N100" s="10"/>
     </row>
-    <row r="101" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="101" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K101" s="10"/>
       <c r="L101" s="10"/>
       <c r="M101" s="10"/>
       <c r="N101" s="10"/>
     </row>
-    <row r="102" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="102" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K102" s="10"/>
       <c r="L102" s="10"/>
       <c r="M102" s="10"/>
       <c r="N102" s="10"/>
     </row>
-    <row r="103" spans="11:14" x14ac:dyDescent="0.45">
+    <row r="103" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K103" s="10"/>
       <c r="L103" s="10"/>
       <c r="M103" s="10"/>
@@ -3326,8 +3732,9 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{FA5862E7-EEED-4C58-B904-536457355E87}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{02BCA972-DCD1-4653-99E4-0BC9A292F8EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>